<commit_message>
get_last_val now stops at blank
</commit_message>
<xml_diff>
--- a/etl_test.xlsx
+++ b/etl_test.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ewanog/code/nepal-earthquake/shelter/etl-extravaganza/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
     <sheet name="Reference" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" calcMode="manual" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
   <si>
     <t>Sourcing Agency</t>
   </si>
@@ -212,6 +217,9 @@
   </si>
   <si>
     <t>notincluded3</t>
+  </si>
+  <si>
+    <t>more</t>
   </si>
 </sst>
 </file>
@@ -418,6 +426,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1014,13 +1027,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:23" ht="61">
+    <row r="1" spans="1:23" ht="66" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -1091,68 +1104,68 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>59</v>
       </c>
       <c r="B12" s="13"/>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -1165,25 +1178,20 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" s="8" customFormat="1" ht="53">
+    <row r="1" spans="1:25" s="8" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>50</v>
       </c>
@@ -1232,109 +1240,107 @@
       <c r="P1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>36</v>
       </c>
+      <c r="S1" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="T1" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="X1" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="Y1" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Y2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>52</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Y3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="Y4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:26">
+      <c r="Y5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>55</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="Y6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>56</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="Y7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>60</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="Y11" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>